<commit_message>
Aggiunti report 19, 20, 21, 23 mar 2022
</commit_message>
<xml_diff>
--- a/dati/rawdata/provinciaCaltanissetta/source/Covid Report 19 Marzo.xlsx
+++ b/dati/rawdata/provinciaCaltanissetta/source/Covid Report 19 Marzo.xlsx
@@ -1,13 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis Angemi\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E19A30ED-95FC-4298-B713-29090611CDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="pr asp" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Foglio3" sheetId="2" r:id="rId5"/>
+    <sheet name="pr asp" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -131,64 +148,67 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-410]d\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="16.0"/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -198,7 +218,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -232,48 +252,74 @@
     </fill>
   </fills>
   <borders count="19">
-    <border/>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -288,8 +334,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -299,14 +347,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -319,6 +371,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -329,6 +382,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -341,12 +395,14 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -359,6 +415,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -371,152 +428,162 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="6" fillId="6" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="13" fillId="6" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="14" fillId="2" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="2" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -674,7 +741,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" w="9525" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -683,13 +750,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="25400" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="38100" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -699,7 +766,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="20000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -708,7 +775,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -717,7 +784,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -727,12 +794,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -763,7 +830,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -782,7 +849,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -794,33 +861,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.43"/>
-    <col customWidth="1" min="2" max="3" width="3.43"/>
-    <col customWidth="1" min="4" max="4" width="20.43"/>
-    <col customWidth="1" min="5" max="5" width="3.43"/>
-    <col customWidth="1" min="6" max="7" width="10.43"/>
-    <col customWidth="1" min="8" max="8" width="11.86"/>
-    <col customWidth="1" min="9" max="10" width="12.86"/>
-    <col customWidth="1" min="11" max="11" width="13.14"/>
-    <col customWidth="1" min="12" max="13" width="10.43"/>
-    <col customWidth="1" min="14" max="14" width="11.43"/>
-    <col customWidth="1" min="15" max="15" width="3.14"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="3" width="3.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" customWidth="1"/>
+    <col min="6" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="14.4">
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" ht="14.4">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -836,7 +904,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:15" ht="23.4">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
@@ -856,7 +924,7 @@
       <c r="N3" s="7"/>
       <c r="O3" s="9"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:15" ht="14.4">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -872,7 +940,7 @@
       <c r="N4" s="7"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:15" ht="21">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -883,7 +951,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12">
-        <v>44639.0</v>
+        <v>44639</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -894,15 +962,15 @@
       <c r="N5" s="14"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:15" ht="15.6">
       <c r="B6" s="6"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -912,739 +980,739 @@
       <c r="N6" s="7"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" ht="54.0" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21" t="s">
+    <row r="7" spans="1:15" ht="54" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="22" t="s">
+      <c r="E7" s="17"/>
+      <c r="F7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="24" t="s">
+      <c r="M7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="26"/>
-    </row>
-    <row r="8">
+      <c r="O7" s="23"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.4">
       <c r="B8" s="6"/>
-      <c r="C8" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29">
-        <v>6.0</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29">
-        <v>145.0</v>
-      </c>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="27" t="str">
-        <f t="shared" ref="N8:N31" si="1">SUM(F8:M8)</f>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26">
+        <v>6</v>
+      </c>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26">
+        <v>145</v>
+      </c>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="24">
+        <f t="shared" ref="N8:N31" si="0">SUM(F8:M8)</f>
         <v>151</v>
       </c>
       <c r="O8" s="9"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:15" ht="14.4">
       <c r="B9" s="6"/>
-      <c r="C9" s="27">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="24">
+        <v>2</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29">
-        <v>78.0</v>
-      </c>
-      <c r="L9" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26">
+        <v>4</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26">
+        <v>78</v>
+      </c>
+      <c r="L9" s="26">
+        <v>1</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="24">
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
       <c r="O9" s="9"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:15" ht="14.4">
       <c r="B10" s="6"/>
-      <c r="C10" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="24">
+        <v>3</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="30">
-        <v>79.0</v>
-      </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="30">
-        <v>555.0</v>
-      </c>
-      <c r="L10" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="27">
+        <v>79</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27">
+        <v>555</v>
+      </c>
+      <c r="L10" s="26">
+        <v>3</v>
+      </c>
+      <c r="M10" s="26"/>
+      <c r="N10" s="24">
+        <f t="shared" si="0"/>
         <v>637</v>
       </c>
       <c r="O10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:15" ht="14.4">
       <c r="B11" s="6"/>
-      <c r="C11" s="27">
-        <v>4.0</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="24">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="30">
-        <v>57.0</v>
-      </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30">
-        <v>514.0</v>
-      </c>
-      <c r="L11" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="27">
+        <v>57</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27">
+        <v>514</v>
+      </c>
+      <c r="L11" s="26">
+        <v>4</v>
+      </c>
+      <c r="M11" s="26"/>
+      <c r="N11" s="24">
+        <f t="shared" si="0"/>
         <v>575</v>
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:15" ht="14.4">
       <c r="B12" s="6"/>
-      <c r="C12" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="24">
+        <v>5</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28">
-        <v>9.0</v>
-      </c>
-      <c r="H12" s="30">
-        <v>1134.0</v>
-      </c>
-      <c r="I12" s="29">
-        <v>2.0</v>
-      </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30">
-        <v>10811.0</v>
-      </c>
-      <c r="L12" s="29">
-        <v>89.0</v>
-      </c>
-      <c r="M12" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="N12" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25">
+        <v>9</v>
+      </c>
+      <c r="H12" s="27">
+        <v>1134</v>
+      </c>
+      <c r="I12" s="26">
+        <v>2</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="27">
+        <v>10811</v>
+      </c>
+      <c r="L12" s="26">
+        <v>89</v>
+      </c>
+      <c r="M12" s="26">
+        <v>1</v>
+      </c>
+      <c r="N12" s="24">
+        <f t="shared" si="0"/>
         <v>12046</v>
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:15" ht="14.4">
       <c r="B13" s="6"/>
-      <c r="C13" s="27">
-        <v>6.0</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="24">
+        <v>6</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="H13" s="30">
-        <v>81.0</v>
-      </c>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="30">
-        <v>545.0</v>
-      </c>
-      <c r="L13" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="M13" s="29"/>
-      <c r="N13" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25">
+        <v>1</v>
+      </c>
+      <c r="H13" s="27">
+        <v>81</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="27">
+        <v>545</v>
+      </c>
+      <c r="L13" s="26">
+        <v>3</v>
+      </c>
+      <c r="M13" s="26"/>
+      <c r="N13" s="24">
+        <f t="shared" si="0"/>
         <v>630</v>
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:15" ht="14.4">
       <c r="B14" s="6"/>
-      <c r="C14" s="27">
-        <v>7.0</v>
-      </c>
-      <c r="D14" s="27" t="s">
+      <c r="C14" s="24">
+        <v>7</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="31">
-        <v>17.0</v>
-      </c>
-      <c r="H14" s="30">
-        <v>1526.0</v>
-      </c>
-      <c r="I14" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30">
-        <v>18004.0</v>
-      </c>
-      <c r="L14" s="29">
-        <v>146.0</v>
-      </c>
-      <c r="M14" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="N14" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="28">
+        <v>17</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1526</v>
+      </c>
+      <c r="I14" s="26">
+        <v>1</v>
+      </c>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27">
+        <v>18004</v>
+      </c>
+      <c r="L14" s="26">
+        <v>146</v>
+      </c>
+      <c r="M14" s="26">
+        <v>1</v>
+      </c>
+      <c r="N14" s="24">
+        <f t="shared" si="0"/>
         <v>19695</v>
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:15" ht="14.4">
       <c r="B15" s="6"/>
-      <c r="C15" s="27">
-        <v>8.0</v>
-      </c>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="24">
+        <v>8</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="30">
-        <v>12.0</v>
-      </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30">
-        <v>304.0</v>
-      </c>
-      <c r="L15" s="29">
-        <v>8.0</v>
-      </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="27">
+        <v>12</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27">
+        <v>304</v>
+      </c>
+      <c r="L15" s="26">
+        <v>8</v>
+      </c>
+      <c r="M15" s="26"/>
+      <c r="N15" s="24">
+        <f t="shared" si="0"/>
         <v>324</v>
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:15" ht="14.4">
       <c r="B16" s="6"/>
-      <c r="C16" s="27">
-        <v>9.0</v>
-      </c>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="24">
+        <v>9</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="H16" s="30">
-        <v>74.0</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30">
-        <v>2236.0</v>
-      </c>
-      <c r="L16" s="29">
-        <v>8.0</v>
-      </c>
-      <c r="M16" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="N16" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25">
+        <v>2</v>
+      </c>
+      <c r="H16" s="27">
+        <v>74</v>
+      </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27">
+        <v>2236</v>
+      </c>
+      <c r="L16" s="26">
+        <v>8</v>
+      </c>
+      <c r="M16" s="26">
+        <v>1</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" si="0"/>
         <v>2321</v>
       </c>
       <c r="O16" s="9"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:17" ht="14.4">
       <c r="B17" s="6"/>
-      <c r="C17" s="27">
-        <v>10.0</v>
-      </c>
-      <c r="D17" s="27" t="s">
+      <c r="C17" s="24">
+        <v>10</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="30">
-        <v>44.0</v>
-      </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30">
-        <v>410.0</v>
-      </c>
-      <c r="L17" s="29">
-        <v>7.0</v>
-      </c>
-      <c r="M17" s="29"/>
-      <c r="N17" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="27">
+        <v>44</v>
+      </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27">
+        <v>410</v>
+      </c>
+      <c r="L17" s="26">
+        <v>7</v>
+      </c>
+      <c r="M17" s="26"/>
+      <c r="N17" s="24">
+        <f t="shared" si="0"/>
         <v>461</v>
       </c>
       <c r="O17" s="9"/>
     </row>
-    <row r="18">
+    <row r="18" spans="2:17" ht="14.4">
       <c r="B18" s="6"/>
-      <c r="C18" s="27">
-        <v>11.0</v>
-      </c>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="24">
+        <v>11</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="30">
-        <v>20.0</v>
-      </c>
-      <c r="I18" s="32"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30">
-        <v>203.0</v>
-      </c>
-      <c r="L18" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="27">
+        <v>20</v>
+      </c>
+      <c r="I18" s="29"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27">
+        <v>203</v>
+      </c>
+      <c r="L18" s="26">
+        <v>4</v>
+      </c>
+      <c r="M18" s="26"/>
+      <c r="N18" s="24">
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
       <c r="O18" s="9"/>
     </row>
-    <row r="19">
+    <row r="19" spans="2:17" ht="14.4">
       <c r="B19" s="6"/>
-      <c r="C19" s="27">
-        <v>12.0</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="24">
+        <v>12</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="30">
-        <v>153.0</v>
-      </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30">
-        <v>1924.0</v>
-      </c>
-      <c r="L19" s="29">
-        <v>12.0</v>
-      </c>
-      <c r="M19" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="N19" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="27">
+        <v>153</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27">
+        <v>1924</v>
+      </c>
+      <c r="L19" s="26">
+        <v>12</v>
+      </c>
+      <c r="M19" s="26">
+        <v>1</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="0"/>
         <v>2090</v>
       </c>
       <c r="O19" s="9"/>
     </row>
-    <row r="20">
+    <row r="20" spans="2:17" ht="14.4">
       <c r="B20" s="6"/>
-      <c r="C20" s="27">
-        <v>13.0</v>
-      </c>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="24">
+        <v>13</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="H20" s="30">
-        <v>243.0</v>
-      </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30">
-        <v>6150.0</v>
-      </c>
-      <c r="L20" s="29">
-        <v>52.0</v>
-      </c>
-      <c r="M20" s="29"/>
-      <c r="N20" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25">
+        <v>1</v>
+      </c>
+      <c r="H20" s="27">
+        <v>243</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27">
+        <v>6150</v>
+      </c>
+      <c r="L20" s="26">
+        <v>52</v>
+      </c>
+      <c r="M20" s="26"/>
+      <c r="N20" s="24">
+        <f t="shared" si="0"/>
         <v>6446</v>
       </c>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="2:17" ht="15.75" customHeight="1">
       <c r="B21" s="6"/>
-      <c r="C21" s="27">
-        <v>14.0</v>
-      </c>
-      <c r="D21" s="27" t="s">
+      <c r="C21" s="24">
+        <v>14</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="H21" s="30">
-        <v>18.0</v>
-      </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29">
-        <v>225.0</v>
-      </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25">
+        <v>1</v>
+      </c>
+      <c r="H21" s="27">
+        <v>18</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26">
+        <v>225</v>
+      </c>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="24">
+        <f t="shared" si="0"/>
         <v>244</v>
       </c>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="2:17" ht="15.75" customHeight="1">
       <c r="B22" s="6"/>
-      <c r="C22" s="27">
-        <v>15.0</v>
-      </c>
-      <c r="D22" s="27" t="s">
+      <c r="C22" s="24">
+        <v>15</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="H22" s="30">
-        <v>76.0</v>
-      </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="30">
-        <v>1737.0</v>
-      </c>
-      <c r="L22" s="29">
-        <v>17.0</v>
-      </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25">
+        <v>1</v>
+      </c>
+      <c r="H22" s="27">
+        <v>76</v>
+      </c>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27">
+        <v>1737</v>
+      </c>
+      <c r="L22" s="26">
+        <v>17</v>
+      </c>
+      <c r="M22" s="26"/>
+      <c r="N22" s="24">
+        <f t="shared" si="0"/>
         <v>1831</v>
       </c>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="2:17" ht="15.75" customHeight="1">
       <c r="B23" s="6"/>
-      <c r="C23" s="27">
-        <v>16.0</v>
-      </c>
-      <c r="D23" s="27" t="s">
+      <c r="C23" s="24">
+        <v>16</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="H23" s="33">
-        <v>454.0</v>
-      </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="30">
-        <v>3662.0</v>
-      </c>
-      <c r="L23" s="29">
-        <v>26.0</v>
-      </c>
-      <c r="M23" s="29"/>
-      <c r="N23" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25">
+        <v>4</v>
+      </c>
+      <c r="H23" s="30">
+        <v>454</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="27">
+        <v>3662</v>
+      </c>
+      <c r="L23" s="26">
+        <v>26</v>
+      </c>
+      <c r="M23" s="26"/>
+      <c r="N23" s="24">
+        <f t="shared" si="0"/>
         <v>4146</v>
       </c>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="2:17" ht="15.75" customHeight="1">
       <c r="B24" s="6"/>
-      <c r="C24" s="27">
-        <v>17.0</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="24">
+        <v>17</v>
+      </c>
+      <c r="D24" s="24" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28">
-        <v>2.0</v>
-      </c>
-      <c r="H24" s="30">
-        <v>95.0</v>
-      </c>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="30">
-        <v>795.0</v>
-      </c>
-      <c r="L24" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="M24" s="29"/>
-      <c r="N24" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25">
+        <v>2</v>
+      </c>
+      <c r="H24" s="27">
+        <v>95</v>
+      </c>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27">
+        <v>795</v>
+      </c>
+      <c r="L24" s="26">
+        <v>4</v>
+      </c>
+      <c r="M24" s="26"/>
+      <c r="N24" s="24">
+        <f t="shared" si="0"/>
         <v>896</v>
       </c>
       <c r="O24" s="9"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="2:17" ht="15.75" customHeight="1">
       <c r="B25" s="6"/>
-      <c r="C25" s="27">
-        <v>18.0</v>
-      </c>
-      <c r="D25" s="27" t="s">
+      <c r="C25" s="24">
+        <v>18</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="31">
-        <v>3.0</v>
-      </c>
-      <c r="H25" s="30">
-        <v>74.0</v>
-      </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="30">
-        <v>922.0</v>
-      </c>
-      <c r="L25" s="29">
-        <v>7.0</v>
-      </c>
-      <c r="M25" s="29"/>
-      <c r="N25" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="28">
+        <v>3</v>
+      </c>
+      <c r="H25" s="27">
+        <v>74</v>
+      </c>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="27">
+        <v>922</v>
+      </c>
+      <c r="L25" s="26">
+        <v>7</v>
+      </c>
+      <c r="M25" s="26"/>
+      <c r="N25" s="24">
+        <f t="shared" si="0"/>
         <v>1006</v>
       </c>
       <c r="O25" s="9"/>
-      <c r="Q25" s="34"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
+      <c r="Q25" s="31"/>
+    </row>
+    <row r="26" spans="2:17" ht="15.75" customHeight="1">
       <c r="B26" s="6"/>
-      <c r="C26" s="27">
-        <v>19.0</v>
-      </c>
-      <c r="D26" s="27" t="s">
+      <c r="C26" s="24">
+        <v>19</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="H26" s="30">
-        <v>209.0</v>
-      </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="30">
-        <v>910.0</v>
-      </c>
-      <c r="L26" s="29">
-        <v>5.0</v>
-      </c>
-      <c r="M26" s="29"/>
-      <c r="N26" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25">
+        <v>1</v>
+      </c>
+      <c r="H26" s="27">
+        <v>209</v>
+      </c>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="27">
+        <v>910</v>
+      </c>
+      <c r="L26" s="26">
+        <v>5</v>
+      </c>
+      <c r="M26" s="26"/>
+      <c r="N26" s="24">
+        <f t="shared" si="0"/>
         <v>1125</v>
       </c>
       <c r="O26" s="9"/>
-      <c r="Q26" s="34"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+      <c r="Q26" s="31"/>
+    </row>
+    <row r="27" spans="2:17" ht="15.75" customHeight="1">
       <c r="B27" s="6"/>
-      <c r="C27" s="27">
-        <v>20.0</v>
-      </c>
-      <c r="D27" s="27" t="s">
+      <c r="C27" s="24">
+        <v>20</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>34</v>
       </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="30">
-        <v>34.0</v>
-      </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="30">
-        <v>84.0</v>
-      </c>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="27">
+        <v>34</v>
+      </c>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="27">
+        <v>84</v>
+      </c>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="24">
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="2:17" ht="15.75" customHeight="1">
       <c r="B28" s="6"/>
-      <c r="C28" s="27">
-        <v>21.0</v>
-      </c>
-      <c r="D28" s="27" t="s">
+      <c r="C28" s="24">
+        <v>21</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="7"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="30">
-        <v>47.0</v>
-      </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="30">
-        <v>732.0</v>
-      </c>
-      <c r="L28" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="27">
+        <v>47</v>
+      </c>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="27">
+        <v>732</v>
+      </c>
+      <c r="L28" s="26">
+        <v>1</v>
+      </c>
+      <c r="M28" s="26"/>
+      <c r="N28" s="24">
+        <f t="shared" si="0"/>
         <v>780</v>
       </c>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="2:17" ht="15.75" customHeight="1">
       <c r="B29" s="6"/>
-      <c r="C29" s="27">
-        <v>22.0</v>
-      </c>
-      <c r="D29" s="27" t="s">
+      <c r="C29" s="24">
+        <v>22</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="30">
-        <v>14.0</v>
-      </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="30">
-        <v>233.0</v>
-      </c>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="27">
+        <v>14</v>
+      </c>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="27">
+        <v>233</v>
+      </c>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="24">
+        <f t="shared" si="0"/>
         <v>247</v>
       </c>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="2:17" ht="15.75" customHeight="1">
       <c r="B30" s="6"/>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37">
-        <v>1.0</v>
-      </c>
-      <c r="G30" s="37">
-        <v>4.0</v>
-      </c>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38">
-        <v>72.0</v>
-      </c>
-      <c r="L30" s="38">
-        <v>37.0</v>
-      </c>
-      <c r="M30" s="38"/>
-      <c r="N30" s="27" t="str">
-        <f t="shared" si="1"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33">
+        <v>1</v>
+      </c>
+      <c r="G30" s="33">
+        <v>4</v>
+      </c>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34">
+        <v>72</v>
+      </c>
+      <c r="L30" s="34">
+        <v>37</v>
+      </c>
+      <c r="M30" s="34"/>
+      <c r="N30" s="24">
+        <f t="shared" si="0"/>
         <v>114</v>
       </c>
       <c r="O30" s="9"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="2:17" ht="15.75" customHeight="1">
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1657,339 +1725,339 @@
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
-      <c r="N31" s="27" t="str">
+      <c r="N31" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B32" s="6"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="37">
+        <f t="shared" ref="F32:M32" si="1">SUM(F8:F30)</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="37">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H32" s="37">
+        <f t="shared" si="1"/>
+        <v>4454</v>
+      </c>
+      <c r="I32" s="37">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J32" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O31" s="9"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="6"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="41" t="str">
-        <f t="shared" ref="F32:M32" si="2">SUM(F8:F30)</f>
-        <v>1</v>
-      </c>
-      <c r="G32" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-      <c r="H32" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>4454</v>
-      </c>
-      <c r="I32" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J32" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="41" t="str">
-        <f t="shared" si="2"/>
+      <c r="K32" s="37">
+        <f t="shared" si="1"/>
         <v>51251</v>
       </c>
-      <c r="L32" s="41" t="str">
-        <f t="shared" si="2"/>
+      <c r="L32" s="37">
+        <f t="shared" si="1"/>
         <v>434</v>
       </c>
-      <c r="M32" s="41" t="str">
-        <f t="shared" si="2"/>
+      <c r="M32" s="37">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="N32" s="27"/>
+      <c r="N32" s="24"/>
       <c r="O32" s="9"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="45"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="33" spans="2:15" ht="15.75" customHeight="1">
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="41"/>
+    </row>
+    <row r="34" spans="2:15" ht="15.75" customHeight="1">
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="2:15" ht="15.75" customHeight="1">
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="2:15" ht="15.75" customHeight="1">
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="2:15" ht="15.75" customHeight="1">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="2:15" ht="15.75" customHeight="1">
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="2:15" ht="15.75" customHeight="1">
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="2:15" ht="15.75" customHeight="1">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="2:15" ht="15.75" customHeight="1">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="2:15" ht="15.75" customHeight="1">
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="2:15" ht="15.75" customHeight="1">
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="2:15" ht="15.75" customHeight="1">
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="2:15" ht="15.75" customHeight="1">
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="2:15" ht="15.75" customHeight="1">
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="2:15" ht="15.75" customHeight="1">
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="2:15" ht="15.75" customHeight="1">
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="6:7" ht="15.75" customHeight="1">
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="6:7" ht="15.75" customHeight="1">
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="6:7" ht="15.75" customHeight="1">
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="6:7" ht="15.75" customHeight="1">
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="6:7" ht="15.75" customHeight="1">
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="6:7" ht="15.75" customHeight="1">
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="6:7" ht="15.75" customHeight="1">
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="6:7" ht="15.75" customHeight="1">
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="6:7" ht="15.75" customHeight="1">
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="6:7" ht="15.75" customHeight="1">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="6:7" ht="15.75" customHeight="1">
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="6:7" ht="15.75" customHeight="1">
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="6:7" ht="15.75" customHeight="1">
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="6:7" ht="15.75" customHeight="1">
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="6:7" ht="15.75" customHeight="1">
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="6:7" ht="15.75" customHeight="1">
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="6:7" ht="15.75" customHeight="1">
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="6:7" ht="15.75" customHeight="1">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="6:7" ht="15.75" customHeight="1">
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="6:7" ht="15.75" customHeight="1">
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="6:7" ht="15.75" customHeight="1">
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="6:7" ht="15.75" customHeight="1">
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="6:7" ht="15.75" customHeight="1">
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="6:7" ht="15.75" customHeight="1">
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="6:7" ht="15.75" customHeight="1">
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="6:7" ht="15.75" customHeight="1">
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="6:7" ht="15.75" customHeight="1">
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="6:7" ht="15.75" customHeight="1">
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="6:7" ht="15.75" customHeight="1">
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="6:7" ht="15.75" customHeight="1">
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="6:7" ht="15.75" customHeight="1">
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="6:7" ht="15.75" customHeight="1">
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="6:7" ht="15.75" customHeight="1">
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="6:7" ht="15.75" customHeight="1">
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="6:7" ht="15.75" customHeight="1">
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="6:7" ht="15.75" customHeight="1">
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="6:7" ht="15.75" customHeight="1">
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="6:7" ht="15.75" customHeight="1">
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="6:7" ht="15.75" customHeight="1">
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="6:7" ht="15.75" customHeight="1">
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="6:7" ht="15.75" customHeight="1">
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="6:7" ht="15.75" customHeight="1">
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="6:7" ht="15.75" customHeight="1">
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="6:7" ht="15.75" customHeight="1">
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="6:7" ht="15.75" customHeight="1">
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="6:7" ht="15.75" customHeight="1">
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="6:7" ht="15.75" customHeight="1">
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="6:7" ht="15.75" customHeight="1">
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="6:7" ht="15.75" customHeight="1">
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="6:7" ht="15.75" customHeight="1">
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="6:7" ht="15.75" customHeight="1">
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="6:7" ht="15.75" customHeight="1">
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
@@ -1998,24 +2066,20 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C30:D30"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A21:A100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="8.86"/>
+    <col min="1" max="6" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2099,9 +2163,7 @@
     <row r="99" ht="15.75" customHeight="1"/>
     <row r="100" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>